<commit_message>
save result to DB
</commit_message>
<xml_diff>
--- a/server/uploads/Toan_6A3_2023_15Phut.xlsx
+++ b/server/uploads/Toan_6A3_2023_15Phut.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Yên Tuấn Phong" sheetId="2" r:id="rId2"/>
+    <sheet name="Vũ Thị Huyền" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -415,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -444,12 +445,23 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="str">
-        <v>04-03-2023 22:40:04</v>
+        <v>05-03-2023 00:23:36</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="str">
+        <v>Vũ Thị Huyền</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <v>05-03-2023 00:27:57</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -564,4 +576,120 @@
     <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="25"/>
+    <col min="2" max="2" customWidth="1" width="25"/>
+    <col min="3" max="3" customWidth="1" width="25"/>
+    <col min="4" max="4" customWidth="1" width="25"/>
+    <col min="5" max="5" customWidth="1" width="8"/>
+    <col min="6" max="6" customWidth="1" width="25"/>
+    <col min="7" max="7" customWidth="1" width="14"/>
+    <col min="8" max="8" customWidth="1" width="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Answer_A</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Answer_B</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Answer_C</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Answer_D</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Num</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>Question</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <v>Answer_Correct</v>
+      </c>
+      <c r="H1" s="3" t="str">
+        <v>Answer_User</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="str">
+        <v>Hyper Text Preprocessor A</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <v>Hyper Text Preprocessor B</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <v>Hyper Text Preprocessor C</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <v>Hyper Text Preprocessor D</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <v>What does HTML stand for?</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <v>Answer_A</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <v>Answer_A</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="str">
+        <v>Hyper Text A</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <v>Hyper Text C</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <v>What does CSS stand for?</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <v>Answer_C</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="str">
+        <v>JavaScript A</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <v>JavaScript B</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <v>JavaScript C</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <v>JavaScript D</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <v>What does JS stand for?</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <v>Answer_A</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>